<commit_message>
Experimenting with Pandas Series
</commit_message>
<xml_diff>
--- a/data/guitar_strings_params - Copy.xlsx
+++ b/data/guitar_strings_params - Copy.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\vcs\git\docs\classical-guitar\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFC880A9-FD0F-41A0-8D11-1D664DFD899F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D1E2DB5-A367-4C8F-9C76-73EF7AA7D874}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="24240" activeTab="2" xr2:uid="{2E890D8E-1EF9-48C8-93AC-046C199C6B8D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="2" xr2:uid="{2E890D8E-1EF9-48C8-93AC-046C199C6B8D}"/>
   </bookViews>
   <sheets>
     <sheet name="EJ43" sheetId="2" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="48">
   <si>
     <t>name</t>
   </si>
@@ -183,9 +183,6 @@
   </si>
   <si>
     <t>J4606FF</t>
-  </si>
-  <si>
-    <t>string</t>
   </si>
 </sst>
 </file>
@@ -561,12 +558,12 @@
   <sheetViews>
     <sheetView zoomScale="200" zoomScaleNormal="200" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="5" max="5" width="10.5703125" customWidth="1"/>
+    <col min="5" max="5" width="10.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -586,7 +583,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -606,7 +603,7 @@
         <v>14.8</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -626,7 +623,7 @@
         <v>11.2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -646,7 +643,7 @@
         <v>11.7</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>21</v>
       </c>
@@ -666,7 +663,7 @@
         <v>14.8</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>22</v>
       </c>
@@ -686,7 +683,7 @@
         <v>12.5</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>23</v>
       </c>
@@ -719,12 +716,12 @@
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="5" max="5" width="10.5703125" customWidth="1"/>
+    <col min="5" max="5" width="10.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -744,7 +741,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>30</v>
       </c>
@@ -764,7 +761,7 @@
         <v>16.399999999999999</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -784,7 +781,7 @@
         <v>12.5</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>32</v>
       </c>
@@ -804,7 +801,7 @@
         <v>12.9</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>33</v>
       </c>
@@ -824,7 +821,7 @@
         <v>16.3</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>34</v>
       </c>
@@ -844,7 +841,7 @@
         <v>15.9</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>35</v>
       </c>
@@ -873,19 +870,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D66F5002-5E53-46DA-A969-797B9E6035D8}">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="5" max="5" width="10.5703125" customWidth="1"/>
+    <col min="5" max="5" width="10.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>48</v>
-      </c>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>16</v>
       </c>
@@ -902,7 +894,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -922,7 +914,7 @@
         <v>15.3</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -942,7 +934,7 @@
         <v>11.6</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -962,7 +954,7 @@
         <v>12.1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -982,7 +974,7 @@
         <v>15.6</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -1002,7 +994,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -1035,12 +1027,12 @@
       <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="5" max="5" width="10.5703125" customWidth="1"/>
+    <col min="5" max="5" width="10.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1060,7 +1052,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>24</v>
       </c>
@@ -1080,7 +1072,7 @@
         <v>15.8</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>25</v>
       </c>
@@ -1100,7 +1092,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>26</v>
       </c>
@@ -1120,7 +1112,7 @@
         <v>12.4</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>27</v>
       </c>
@@ -1140,7 +1132,7 @@
         <v>16.3</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>28</v>
       </c>
@@ -1160,7 +1152,7 @@
         <v>15.9</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>29</v>
       </c>
@@ -1193,12 +1185,12 @@
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="5" max="5" width="10.5703125" customWidth="1"/>
+    <col min="5" max="5" width="10.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1218,7 +1210,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>36</v>
       </c>
@@ -1238,7 +1230,7 @@
         <v>21.29</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>37</v>
       </c>
@@ -1258,7 +1250,7 @@
         <v>15.35</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>38</v>
       </c>
@@ -1278,7 +1270,7 @@
         <v>14.32</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>39</v>
       </c>
@@ -1298,7 +1290,7 @@
         <v>13.64</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>40</v>
       </c>
@@ -1318,7 +1310,7 @@
         <v>14.7</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>41</v>
       </c>
@@ -1351,12 +1343,12 @@
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="5" max="5" width="10.5703125" customWidth="1"/>
+    <col min="5" max="5" width="10.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1376,7 +1368,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>42</v>
       </c>
@@ -1396,7 +1388,7 @@
         <v>22.74</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>43</v>
       </c>
@@ -1416,7 +1408,7 @@
         <v>16.27</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>44</v>
       </c>
@@ -1436,7 +1428,7 @@
         <v>15.02</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>45</v>
       </c>
@@ -1456,7 +1448,7 @@
         <v>15.28</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>46</v>
       </c>
@@ -1476,7 +1468,7 @@
         <v>16.97</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>47</v>
       </c>

</xml_diff>

<commit_message>
Updated params data file format
</commit_message>
<xml_diff>
--- a/data/guitar_strings_params - Copy.xlsx
+++ b/data/guitar_strings_params - Copy.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\vcs\git\docs\classical-guitar\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D1E2DB5-A367-4C8F-9C76-73EF7AA7D874}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05B007B1-36EC-4AB3-BD43-D025F4F391DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="2" xr2:uid="{2E890D8E-1EF9-48C8-93AC-046C199C6B8D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="5" xr2:uid="{2E890D8E-1EF9-48C8-93AC-046C199C6B8D}"/>
   </bookViews>
   <sheets>
     <sheet name="EJ43" sheetId="2" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="48">
   <si>
     <t>name</t>
   </si>
@@ -556,31 +556,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E08288C-F451-488C-ADF5-051FF7808691}">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView zoomScale="200" zoomScaleNormal="200" workbookViewId="0"/>
+    <sheetView zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="5" max="5" width="10.5546875" customWidth="1"/>
+    <col min="4" max="4" width="10.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
       <c r="B1" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -590,17 +589,17 @@
       <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="1">
-        <v>25.5</v>
-      </c>
-      <c r="D2" s="2">
+      <c r="C2" s="2">
         <v>2.75E-2</v>
       </c>
-      <c r="E2" s="3">
+      <c r="D2" s="3">
         <v>2.0239999999999999E-5</v>
       </c>
-      <c r="F2" s="4">
+      <c r="E2" s="4">
         <v>14.8</v>
+      </c>
+      <c r="F2" s="1">
+        <v>25.5</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -610,17 +609,17 @@
       <c r="B3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="1">
-        <v>25.5</v>
-      </c>
-      <c r="D3" s="2">
+      <c r="C3" s="2">
         <v>3.1699999999999999E-2</v>
       </c>
-      <c r="E3" s="3">
+      <c r="D3" s="3">
         <v>2.7290000000000001E-5</v>
       </c>
-      <c r="F3" s="4">
+      <c r="E3" s="4">
         <v>11.2</v>
+      </c>
+      <c r="F3" s="1">
+        <v>25.5</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -630,17 +629,17 @@
       <c r="B4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="1">
-        <v>25.5</v>
-      </c>
-      <c r="D4" s="2">
+      <c r="C4" s="2">
         <v>3.9699999999999999E-2</v>
       </c>
-      <c r="E4" s="3">
+      <c r="D4" s="3">
         <v>4.5250000000000002E-5</v>
       </c>
-      <c r="F4" s="4">
+      <c r="E4" s="4">
         <v>11.7</v>
+      </c>
+      <c r="F4" s="1">
+        <v>25.5</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -650,17 +649,17 @@
       <c r="B5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="1">
-        <v>25.5</v>
-      </c>
-      <c r="D5" s="2">
+      <c r="C5" s="2">
         <v>2.8000000000000001E-2</v>
       </c>
-      <c r="E5" s="3">
+      <c r="D5" s="3">
         <v>1.0203E-4</v>
       </c>
-      <c r="F5" s="4">
+      <c r="E5" s="4">
         <v>14.8</v>
+      </c>
+      <c r="F5" s="1">
+        <v>25.5</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -670,17 +669,17 @@
       <c r="B6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="1">
-        <v>25.5</v>
-      </c>
-      <c r="D6" s="2">
+      <c r="C6" s="2">
         <v>3.3000000000000002E-2</v>
       </c>
-      <c r="E6" s="3">
+      <c r="D6" s="3">
         <v>1.5347000000000001E-4</v>
       </c>
-      <c r="F6" s="4">
+      <c r="E6" s="4">
         <v>12.5</v>
+      </c>
+      <c r="F6" s="1">
+        <v>25.5</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -690,17 +689,17 @@
       <c r="B7" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="1">
-        <v>25.5</v>
-      </c>
-      <c r="D7" s="2">
+      <c r="C7" s="2">
         <v>4.2000000000000003E-2</v>
       </c>
-      <c r="E7" s="3">
+      <c r="D7" s="3">
         <v>2.8881000000000002E-4</v>
       </c>
-      <c r="F7" s="4">
+      <c r="E7" s="4">
         <v>13.2</v>
+      </c>
+      <c r="F7" s="1">
+        <v>25.5</v>
       </c>
     </row>
   </sheetData>
@@ -713,32 +712,29 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="5" max="5" width="10.5546875" customWidth="1"/>
+    <col min="4" max="4" width="10.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
       <c r="B1" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -748,17 +744,17 @@
       <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="1">
-        <v>25.5</v>
-      </c>
-      <c r="D2" s="2">
+      <c r="C2" s="2">
         <v>2.9000000000000001E-2</v>
       </c>
-      <c r="E2" s="3">
+      <c r="D2" s="3">
         <v>2.243E-5</v>
       </c>
-      <c r="F2" s="4">
+      <c r="E2" s="4">
         <v>16.399999999999999</v>
+      </c>
+      <c r="F2" s="1">
+        <v>25.5</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -768,17 +764,17 @@
       <c r="B3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="1">
-        <v>25.5</v>
-      </c>
-      <c r="D3" s="2">
+      <c r="C3" s="2">
         <v>3.3300000000000003E-2</v>
       </c>
-      <c r="E3" s="3">
+      <c r="D3" s="3">
         <v>3.046E-5</v>
       </c>
-      <c r="F3" s="4">
+      <c r="E3" s="4">
         <v>12.5</v>
+      </c>
+      <c r="F3" s="1">
+        <v>25.5</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -788,17 +784,17 @@
       <c r="B4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="1">
-        <v>25.5</v>
-      </c>
-      <c r="D4" s="2">
+      <c r="C4" s="2">
         <v>4.1599999999999998E-2</v>
       </c>
-      <c r="E4" s="3">
+      <c r="D4" s="3">
         <v>4.9889999999999998E-5</v>
       </c>
-      <c r="F4" s="4">
+      <c r="E4" s="4">
         <v>12.9</v>
+      </c>
+      <c r="F4" s="1">
+        <v>25.5</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -808,17 +804,17 @@
       <c r="B5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="1">
-        <v>25.5</v>
-      </c>
-      <c r="D5" s="2">
+      <c r="C5" s="2">
         <v>0.03</v>
       </c>
-      <c r="E5" s="3">
+      <c r="D5" s="3">
         <v>1.1237E-4</v>
       </c>
-      <c r="F5" s="4">
+      <c r="E5" s="4">
         <v>16.3</v>
+      </c>
+      <c r="F5" s="1">
+        <v>25.5</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -828,17 +824,17 @@
       <c r="B6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="1">
-        <v>25.5</v>
-      </c>
-      <c r="D6" s="2">
+      <c r="C6" s="2">
         <v>3.5999999999999997E-2</v>
       </c>
-      <c r="E6" s="3">
+      <c r="D6" s="3">
         <v>1.9521E-4</v>
       </c>
-      <c r="F6" s="4">
+      <c r="E6" s="4">
         <v>15.9</v>
+      </c>
+      <c r="F6" s="1">
+        <v>25.5</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -848,17 +844,17 @@
       <c r="B7" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="1">
-        <v>25.5</v>
-      </c>
-      <c r="D7" s="2">
+      <c r="C7" s="2">
         <v>4.4999999999999998E-2</v>
       </c>
-      <c r="E7" s="3">
+      <c r="D7" s="3">
         <v>3.4351E-4</v>
       </c>
-      <c r="F7" s="4">
+      <c r="E7" s="4">
         <v>15.7</v>
+      </c>
+      <c r="F7" s="1">
+        <v>25.5</v>
       </c>
     </row>
   </sheetData>
@@ -870,11 +866,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D66F5002-5E53-46DA-A969-797B9E6035D8}">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0"/>
+    <sheetView zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="5" max="5" width="10.5546875" customWidth="1"/>
+    <col min="4" max="4" width="10.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
@@ -882,16 +880,16 @@
         <v>16</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -901,17 +899,17 @@
       <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="1">
-        <v>25.5</v>
-      </c>
-      <c r="D2" s="2">
+      <c r="C2" s="2">
         <v>2.8000000000000001E-2</v>
       </c>
-      <c r="E2" s="3">
+      <c r="D2" s="3">
         <v>2.092E-5</v>
       </c>
-      <c r="F2" s="4">
+      <c r="E2" s="4">
         <v>15.3</v>
+      </c>
+      <c r="F2" s="1">
+        <v>25.5</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -921,17 +919,17 @@
       <c r="B3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="1">
-        <v>25.5</v>
-      </c>
-      <c r="D3" s="2">
+      <c r="C3" s="2">
         <v>3.2199999999999999E-2</v>
       </c>
-      <c r="E3" s="3">
+      <c r="D3" s="3">
         <v>2.8269999999999999E-5</v>
       </c>
-      <c r="F3" s="4">
+      <c r="E3" s="4">
         <v>11.6</v>
+      </c>
+      <c r="F3" s="1">
+        <v>25.5</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -941,17 +939,17 @@
       <c r="B4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="1">
-        <v>25.5</v>
-      </c>
-      <c r="D4" s="2">
+      <c r="C4" s="2">
         <v>4.0300000000000002E-2</v>
       </c>
-      <c r="E4" s="3">
+      <c r="D4" s="3">
         <v>4.6789999999999998E-5</v>
       </c>
-      <c r="F4" s="4">
+      <c r="E4" s="4">
         <v>12.1</v>
+      </c>
+      <c r="F4" s="1">
+        <v>25.5</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -961,17 +959,17 @@
       <c r="B5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="1">
-        <v>25.5</v>
-      </c>
-      <c r="D5" s="2">
+      <c r="C5" s="2">
         <v>2.9000000000000001E-2</v>
       </c>
-      <c r="E5" s="3">
+      <c r="D5" s="3">
         <v>1.0754E-4</v>
       </c>
-      <c r="F5" s="4">
+      <c r="E5" s="4">
         <v>15.6</v>
+      </c>
+      <c r="F5" s="1">
+        <v>25.5</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -981,17 +979,17 @@
       <c r="B6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="1">
-        <v>25.5</v>
-      </c>
-      <c r="D6" s="2">
+      <c r="C6" s="2">
         <v>3.5000000000000003E-2</v>
       </c>
-      <c r="E6" s="3">
+      <c r="D6" s="3">
         <v>1.8416E-4</v>
       </c>
-      <c r="F6" s="4">
+      <c r="E6" s="4">
         <v>15</v>
+      </c>
+      <c r="F6" s="1">
+        <v>25.5</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -1001,17 +999,17 @@
       <c r="B7" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="1">
-        <v>25.5</v>
-      </c>
-      <c r="D7" s="2">
+      <c r="C7" s="2">
         <v>4.2999999999999997E-2</v>
       </c>
-      <c r="E7" s="3">
+      <c r="D7" s="3">
         <v>3.0632000000000001E-4</v>
       </c>
-      <c r="F7" s="4">
+      <c r="E7" s="4">
         <v>14</v>
+      </c>
+      <c r="F7" s="1">
+        <v>25.5</v>
       </c>
     </row>
   </sheetData>
@@ -1024,32 +1022,29 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="5" max="5" width="10.5546875" customWidth="1"/>
+    <col min="4" max="4" width="10.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
       <c r="B1" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -1059,17 +1054,17 @@
       <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="1">
-        <v>25.5</v>
-      </c>
-      <c r="D2" s="2">
+      <c r="C2" s="2">
         <v>2.8500000000000001E-2</v>
       </c>
-      <c r="E2" s="3">
+      <c r="D2" s="3">
         <v>2.1610000000000001E-5</v>
       </c>
-      <c r="F2" s="4">
+      <c r="E2" s="4">
         <v>15.8</v>
+      </c>
+      <c r="F2" s="1">
+        <v>25.5</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -1079,17 +1074,17 @@
       <c r="B3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="1">
-        <v>25.5</v>
-      </c>
-      <c r="D3" s="2">
+      <c r="C3" s="2">
         <v>3.27E-2</v>
       </c>
-      <c r="E3" s="3">
+      <c r="D3" s="3">
         <v>2.9240000000000001E-5</v>
       </c>
-      <c r="F3" s="4">
+      <c r="E3" s="4">
         <v>12</v>
+      </c>
+      <c r="F3" s="1">
+        <v>25.5</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -1099,17 +1094,17 @@
       <c r="B4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="1">
-        <v>25.5</v>
-      </c>
-      <c r="D4" s="2">
+      <c r="C4" s="2">
         <v>4.1000000000000002E-2</v>
       </c>
-      <c r="E4" s="3">
+      <c r="D4" s="3">
         <v>4.795E-5</v>
       </c>
-      <c r="F4" s="4">
+      <c r="E4" s="4">
         <v>12.4</v>
+      </c>
+      <c r="F4" s="1">
+        <v>25.5</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -1119,17 +1114,17 @@
       <c r="B5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="1">
-        <v>25.5</v>
-      </c>
-      <c r="D5" s="2">
+      <c r="C5" s="2">
         <v>0.03</v>
       </c>
-      <c r="E5" s="3">
+      <c r="D5" s="3">
         <v>1.1237E-4</v>
       </c>
-      <c r="F5" s="4">
+      <c r="E5" s="4">
         <v>16.3</v>
+      </c>
+      <c r="F5" s="1">
+        <v>25.5</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -1139,17 +1134,17 @@
       <c r="B6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="1">
-        <v>25.5</v>
-      </c>
-      <c r="D6" s="2">
+      <c r="C6" s="2">
         <v>3.5999999999999997E-2</v>
       </c>
-      <c r="E6" s="3">
+      <c r="D6" s="3">
         <v>1.9521E-4</v>
       </c>
-      <c r="F6" s="4">
+      <c r="E6" s="4">
         <v>15.9</v>
+      </c>
+      <c r="F6" s="1">
+        <v>25.5</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -1159,17 +1154,17 @@
       <c r="B7" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="1">
-        <v>25.5</v>
-      </c>
-      <c r="D7" s="2">
+      <c r="C7" s="2">
         <v>4.3999999999999997E-2</v>
       </c>
-      <c r="E7" s="3">
+      <c r="D7" s="3">
         <v>3.1725999999999998E-4</v>
       </c>
-      <c r="F7" s="4">
+      <c r="E7" s="4">
         <v>14.5</v>
+      </c>
+      <c r="F7" s="1">
+        <v>25.5</v>
       </c>
     </row>
   </sheetData>
@@ -1182,32 +1177,29 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="5" max="5" width="10.5546875" customWidth="1"/>
+    <col min="4" max="4" width="10.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
       <c r="B1" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -1217,17 +1209,17 @@
       <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="1">
-        <v>25.5</v>
-      </c>
-      <c r="D2" s="2">
+      <c r="C2" s="2">
         <v>2.4E-2</v>
       </c>
-      <c r="E2" s="3">
+      <c r="D2" s="3">
         <v>2.5999999999999998E-5</v>
       </c>
-      <c r="F2" s="5">
+      <c r="E2" s="5">
         <v>21.29</v>
+      </c>
+      <c r="F2" s="1">
+        <v>25.5</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -1237,17 +1229,17 @@
       <c r="B3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="1">
-        <v>25.5</v>
-      </c>
-      <c r="D3" s="2">
+      <c r="C3" s="2">
         <v>2.7199999999999998E-2</v>
       </c>
-      <c r="E3" s="3">
+      <c r="D3" s="3">
         <v>3.4E-5</v>
       </c>
-      <c r="F3" s="5">
+      <c r="E3" s="5">
         <v>15.35</v>
+      </c>
+      <c r="F3" s="1">
+        <v>25.5</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -1257,17 +1249,17 @@
       <c r="B4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="1">
-        <v>25.5</v>
-      </c>
-      <c r="D4" s="2">
+      <c r="C4" s="2">
         <v>3.3099999999999997E-2</v>
       </c>
-      <c r="E4" s="3">
+      <c r="D4" s="3">
         <v>5.0000000000000002E-5</v>
       </c>
-      <c r="F4" s="5">
+      <c r="E4" s="5">
         <v>14.32</v>
+      </c>
+      <c r="F4" s="1">
+        <v>25.5</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -1277,17 +1269,17 @@
       <c r="B5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="1">
-        <v>25.5</v>
-      </c>
-      <c r="D5" s="2">
+      <c r="C5" s="2">
         <v>2.8000000000000001E-2</v>
       </c>
-      <c r="E5" s="3">
+      <c r="D5" s="3">
         <v>9.2E-5</v>
       </c>
-      <c r="F5" s="5">
+      <c r="E5" s="5">
         <v>13.64</v>
+      </c>
+      <c r="F5" s="1">
+        <v>25.5</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -1297,17 +1289,17 @@
       <c r="B6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="1">
-        <v>25.5</v>
-      </c>
-      <c r="D6" s="2">
+      <c r="C6" s="2">
         <v>3.5000000000000003E-2</v>
       </c>
-      <c r="E6" s="3">
+      <c r="D6" s="3">
         <v>1.73E-4</v>
       </c>
-      <c r="F6" s="5">
+      <c r="E6" s="5">
         <v>14.7</v>
+      </c>
+      <c r="F6" s="1">
+        <v>25.5</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -1317,17 +1309,17 @@
       <c r="B7" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="1">
-        <v>25.5</v>
-      </c>
-      <c r="D7" s="2">
+      <c r="C7" s="2">
         <v>4.3999999999999997E-2</v>
       </c>
-      <c r="E7" s="3">
+      <c r="D7" s="3">
         <v>3.2000000000000003E-4</v>
       </c>
-      <c r="F7" s="5">
+      <c r="E7" s="5">
         <v>15.25</v>
+      </c>
+      <c r="F7" s="1">
+        <v>25.5</v>
       </c>
     </row>
   </sheetData>
@@ -1339,13 +1331,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27F174DE-CC2E-4D4C-A29D-1F98FEBEDE90}">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="5" max="5" width="10.5546875" customWidth="1"/>
+    <col min="4" max="4" width="10.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
@@ -1356,16 +1348,16 @@
         <v>16</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -1375,17 +1367,17 @@
       <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="1">
-        <v>25.5</v>
-      </c>
-      <c r="D2" s="2">
+      <c r="C2" s="2">
         <v>2.4799999999999999E-2</v>
       </c>
-      <c r="E2" s="3">
+      <c r="D2" s="3">
         <v>2.8E-5</v>
       </c>
-      <c r="F2" s="5">
+      <c r="E2" s="5">
         <v>22.74</v>
+      </c>
+      <c r="F2" s="1">
+        <v>25.5</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -1395,17 +1387,17 @@
       <c r="B3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="1">
-        <v>25.5</v>
-      </c>
-      <c r="D3" s="2">
+      <c r="C3" s="2">
         <v>2.8000000000000001E-2</v>
       </c>
-      <c r="E3" s="3">
+      <c r="D3" s="3">
         <v>3.6000000000000001E-5</v>
       </c>
-      <c r="F3" s="5">
+      <c r="E3" s="5">
         <v>16.27</v>
+      </c>
+      <c r="F3" s="1">
+        <v>25.5</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -1415,17 +1407,17 @@
       <c r="B4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="1">
-        <v>25.5</v>
-      </c>
-      <c r="D4" s="2">
+      <c r="C4" s="2">
         <v>3.39E-2</v>
       </c>
-      <c r="E4" s="3">
+      <c r="D4" s="3">
         <v>5.3000000000000001E-5</v>
       </c>
-      <c r="F4" s="5">
+      <c r="E4" s="5">
         <v>15.02</v>
+      </c>
+      <c r="F4" s="1">
+        <v>25.5</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -1435,17 +1427,17 @@
       <c r="B5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="1">
-        <v>25.5</v>
-      </c>
-      <c r="D5" s="2">
+      <c r="C5" s="2">
         <v>2.9000000000000001E-2</v>
       </c>
-      <c r="E5" s="3">
+      <c r="D5" s="3">
         <v>1.03E-4</v>
       </c>
-      <c r="F5" s="5">
+      <c r="E5" s="5">
         <v>15.28</v>
+      </c>
+      <c r="F5" s="1">
+        <v>25.5</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -1455,17 +1447,17 @@
       <c r="B6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="1">
-        <v>25.5</v>
-      </c>
-      <c r="D6" s="2">
+      <c r="C6" s="2">
         <v>3.5999999999999997E-2</v>
       </c>
-      <c r="E6" s="3">
+      <c r="D6" s="3">
         <v>1.9900000000000001E-4</v>
       </c>
-      <c r="F6" s="5">
+      <c r="E6" s="5">
         <v>16.97</v>
+      </c>
+      <c r="F6" s="1">
+        <v>25.5</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -1475,17 +1467,17 @@
       <c r="B7" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="1">
-        <v>25.5</v>
-      </c>
-      <c r="D7" s="2">
+      <c r="C7" s="2">
         <v>4.5999999999999999E-2</v>
       </c>
-      <c r="E7" s="3">
+      <c r="D7" s="3">
         <v>3.4299999999999999E-4</v>
       </c>
-      <c r="F7" s="5">
+      <c r="E7" s="5">
         <v>16.36</v>
+      </c>
+      <c r="F7" s="1">
+        <v>25.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Moving GuitarString and GuitarStrings to all-Pandas-all-the-time
Danger! Unstable!
</commit_message>
<xml_diff>
--- a/data/guitar_strings_params - Copy.xlsx
+++ b/data/guitar_strings_params - Copy.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\vcs\git\docs\classical-guitar\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05B007B1-36EC-4AB3-BD43-D025F4F391DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22A84EF8-8324-4628-8399-A3E038FA9BC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="5" xr2:uid="{2E890D8E-1EF9-48C8-93AC-046C199C6B8D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="2" xr2:uid="{2E890D8E-1EF9-48C8-93AC-046C199C6B8D}"/>
   </bookViews>
   <sheets>
     <sheet name="EJ43" sheetId="2" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="49">
   <si>
     <t>name</t>
   </si>
@@ -183,6 +183,9 @@
   </si>
   <si>
     <t>J4606FF</t>
+  </si>
+  <si>
+    <t>string</t>
   </si>
 </sst>
 </file>
@@ -866,9 +869,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D66F5002-5E53-46DA-A969-797B9E6035D8}">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -876,6 +877,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>48</v>
+      </c>
       <c r="B1" s="1" t="s">
         <v>16</v>
       </c>
@@ -1331,7 +1335,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27F174DE-CC2E-4D4C-A29D-1F98FEBEDE90}">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+    <sheetView zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>

</xml_diff>